<commit_message>
Added all 8 pie slices at Roth Tech Farm
</commit_message>
<xml_diff>
--- a/travis/kcb/kcb_import_control.xlsx
+++ b/travis/kcb/kcb_import_control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztz\github_projects\sharda_python_practice\travis\kcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12B73BB-8E46-46ED-949E-A20D4BF01CA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517C9CF4-855F-4E10-A47D-157658DFE14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82A72517-AA17-40E6-BEC4-01AC68791A74}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{82A72517-AA17-40E6-BEC4-01AC68791A74}"/>
   </bookViews>
   <sheets>
     <sheet name="config_1" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>longitude in decimal degrees (wgs84)</t>
-  </si>
-  <si>
     <t>2 digit prefix to use for naming weather stations (e.g. 'OW' will produce weather stations named OW01, OW02, OW03 … for the individual csv files found)</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>out_directory</t>
   </si>
   <si>
-    <t>LN</t>
-  </si>
-  <si>
     <t>date_col</t>
   </si>
   <si>
@@ -161,6 +155,12 @@
   </si>
   <si>
     <t>Directoryt to store file</t>
+  </si>
+  <si>
+    <t>Column to use for KCB (starting at 0,1,2,….)</t>
+  </si>
+  <si>
+    <t>RT</t>
   </si>
 </sst>
 </file>
@@ -606,7 +606,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.7"/>
@@ -624,7 +624,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -640,57 +640,57 @@
     </row>
     <row r="5" spans="1:3" ht="29.4">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>38</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="14">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15">
@@ -726,18 +726,18 @@
     <row r="2" spans="1:3" s="10" customFormat="1"/>
     <row r="3" spans="1:3" ht="18.3">
       <c r="A3" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.7">
@@ -745,10 +745,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.7">
@@ -756,84 +756,84 @@
     </row>
     <row r="7" spans="1:3" ht="18.3">
       <c r="A7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -843,12 +843,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1075,15 +1072,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18EE1BDF-624F-4413-84BE-165990F9E7E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A174D336-94B7-4ECB-97E3-C87513CDE339}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="0b9de3d3-35f4-4d75-b390-47a360cdbec9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f623e1fa-06c0-442c-bf13-6b417fbd2da3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1108,18 +1117,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A174D336-94B7-4ECB-97E3-C87513CDE339}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18EE1BDF-624F-4413-84BE-165990F9E7E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="0b9de3d3-35f4-4d75-b390-47a360cdbec9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f623e1fa-06c0-442c-bf13-6b417fbd2da3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>